<commit_message>
chore completed upload form UI
</commit_message>
<xml_diff>
--- a/src/assets/document/QUESTION_TEMPLATE.xlsx
+++ b/src/assets/document/QUESTION_TEMPLATE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdammyy/Development/Web/ipcm-web/src/assets/document/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdammyy/Development/codeBase/Web/ipcm-web/src/assets/document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17124DD-03E0-E04E-8547-504BA06A004D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9AD49F-2D6B-754D-BCC3-1D7313D24E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3020" yWindow="2920" windowWidth="28040" windowHeight="17440" xr2:uid="{57979201-6F4B-6B44-A4C7-F5C64AFF8A91}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Serial_Number</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -45,7 +42,10 @@
     <t>answer</t>
   </si>
   <si>
-    <t>Question</t>
+    <t>question</t>
+  </si>
+  <si>
+    <t>qstNumber</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -421,25 +421,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>